<commit_message>
add bundle in data init
</commit_message>
<xml_diff>
--- a/src/main/resources/Question-Tekor.xlsx
+++ b/src/main/resources/Question-Tekor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\Class\final_project\backend\tekor\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F291BE0-CED2-4757-AE15-85E20E13816C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF7050E-715E-4C2A-9965-9043072EE90F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{8797CD74-DAE5-4304-B1C3-CC355A84F94F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="222">
   <si>
     <t>LISTENING</t>
   </si>
@@ -408,9 +408,6 @@
     <t>빗자루와 쓰레받기를 이용하여 청소하고 있습니다.</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dtxx1gcip/video/upload/v1751795585/ciszcigvydhcafh6wli9.mp3</t>
-  </si>
-  <si>
     <t>우유</t>
   </si>
   <si>
@@ -423,9 +420,6 @@
     <t>이유</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/dtxx1gcip/video/upload/v1751795585/vy6cnt2rlksqs7cqpfom.mp3</t>
-  </si>
-  <si>
     <t>아깝습니다</t>
   </si>
   <si>
@@ -637,6 +631,72 @@
   </si>
   <si>
     <t>desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  문제입니다 오이</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  문제입니다  가깝습니다</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  문제입니다  가방을 맡기세요</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  문제입니다  우리 가족은 모두 6 명이에요.</t>
+  </si>
+  <si>
+    <t>1번, 식사를 하고 있습니다. 2번, 빨래를 하고 있습니다. 3번, 머리를 자르고 있습니다.  4번, 김치를 만들고 있습니다</t>
+  </si>
+  <si>
+    <t>1번, 신문입니다. 2번, 책상입니다. 3번, 연필입니다. 4번, 가방입니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1번, 간호사입니다. 2번, 미용사입니다. 3번, 요리사입니다. 4번, 운전기사입니다.</t>
+  </si>
+  <si>
+    <t>1번, 1월 3일입니다. 2번, 1월 30일입니다. 3번, 2월 3일입니다. 4번, 3월 10일입니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1번, 흐립니다. 2번, 막습니다. 3번, 눈이 옵니다. 4번, 비가 옵니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 몇 시에 일어납니까? 6시에 일어납니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 우리 가족은 모두 5명입니다. 할머니, 아버지, 어머니, 언니, 그리고 저입니다. 아빠만 남자이고 모두 여자입니다.</t>
+  </si>
+  <si>
+    <t>사무실에서 담배를 피워도 돼요? 아니요. 사무실에서 담배 피우면 안 돼요.</t>
+  </si>
+  <si>
+    <t>문제입니다. 얀또씨가 누구예요? 1번. 제가 얀또입니다. 2번. 얀또씨 책이에요. 3번.어제 구두를 샀어요. 4번. 인도네시아에서 왔어요.</t>
+  </si>
+  <si>
+    <t>문제입니다. 언제 만날까요? 1번. 친구를 만날 거예요. 2번. 이번 토요일에 만나요. 3번.작년에 한국에 왔어요. 4번. 한국 식당에서 먹어요.</t>
+  </si>
+  <si>
+    <t>문제입니다. 여기서 공항까지 어떻게 가요? 1번. 공항 버스를 타면 돼요. 2번. 회사 일 때문에 출장 가요. 3번. 캄보디아에서 친구가 올 거예요. 4번. 3시까지 공항에 도착해야 해요.</t>
+  </si>
+  <si>
+    <t>문제입니다. 뭘 마시겠어요? 1번. 제가 만들겠어요. 2번. 주스를 마시겠어요. 3번. 식당에서 먹겠어요. 4번. 한국말을 배우겠어요.</t>
+  </si>
+  <si>
+    <t>문제입니다. 날마다 한국어 학원에 가요? 1번. 아니요. 다음 달에 한국에 가요. 2번. 아니요.날마다 한국말을 공부해요. 3번. 아니요.오후 2시부터 4시까지예요. 4번. 아니요.</t>
+  </si>
+  <si>
+    <t>문제입니다. 실례지만 한국 사람입니까? 아니요. 한국 사람이 아니에요. 몽골 사람이에요. 그래요? 그런데 한국말을 참 잘하시네요</t>
+  </si>
+  <si>
+    <t>내일 7시에 저녁을 같이 먹어요. 그 시간에는 텔레비전을 봐야 해요. 한국 드라마를 하거든요. 몇 시에 하는데요? 7시요. 오후 7시부터 8시까지 해요. 그럼 9시에 만납시다. 네. 그래요.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 문제입니다. 2번역이 시청역이지요? 아니요. 다음역이 시청역이에요. 그럼 우리 다음역에서 내려서 1호선으로 갈아타야 해요</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dtxx1gcip/video/upload/v1751866385/jlgw6tbjo9k4nkqagdu1.mp3</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/dtxx1gcip/video/upload/v1751866705/27new_dtkoam.mp3</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372CAD71-1847-4062-9898-090013898285}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1065,12 +1125,13 @@
     <col min="1" max="1" width="58.54296875" customWidth="1"/>
     <col min="2" max="2" width="25.26953125" customWidth="1"/>
     <col min="3" max="3" width="34.81640625" customWidth="1"/>
-    <col min="4" max="4" width="39.26953125" customWidth="1"/>
+    <col min="4" max="4" width="82.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.453125" customWidth="1"/>
     <col min="6" max="6" width="31.81640625" customWidth="1"/>
     <col min="7" max="7" width="24.7265625" customWidth="1"/>
     <col min="8" max="8" width="22.26953125" customWidth="1"/>
     <col min="9" max="9" width="43.6328125" customWidth="1"/>
+    <col min="10" max="10" width="159.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
@@ -1102,7 +1163,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
@@ -1642,24 +1703,26 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="I22" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J22" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
@@ -1668,24 +1731,26 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="I23" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="J23" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
@@ -1694,24 +1759,26 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="I24" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J24" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
@@ -1720,28 +1787,30 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="I25" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="J25" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>0</v>
@@ -1750,7 +1819,7 @@
         <v>29</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
@@ -1767,11 +1836,13 @@
       <c r="I26" s="1">
         <v>4</v>
       </c>
-      <c r="J26" s="1"/>
+      <c r="J26" s="1" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>0</v>
@@ -1780,7 +1851,7 @@
         <v>30</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
@@ -1797,11 +1868,13 @@
       <c r="I27" s="1">
         <v>1</v>
       </c>
-      <c r="J27" s="1"/>
+      <c r="J27" s="1" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>0</v>
@@ -1810,7 +1883,7 @@
         <v>31</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
@@ -1827,11 +1900,13 @@
       <c r="I28" s="1">
         <v>2</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>0</v>
@@ -1840,7 +1915,7 @@
         <v>32</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
@@ -1857,11 +1932,13 @@
       <c r="I29" s="1">
         <v>2</v>
       </c>
-      <c r="J29" s="1"/>
+      <c r="J29" s="1" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>0</v>
@@ -1870,7 +1947,7 @@
         <v>33</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -1887,7 +1964,9 @@
       <c r="I30" s="1">
         <v>2</v>
       </c>
-      <c r="J30" s="1"/>
+      <c r="J30" s="1" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
@@ -1896,7 +1975,7 @@
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>34</v>
@@ -1913,7 +1992,9 @@
       <c r="I31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J31" s="1"/>
+      <c r="J31" s="1" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
@@ -1922,7 +2003,7 @@
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>38</v>
@@ -1939,7 +2020,9 @@
       <c r="I32" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J32" s="1"/>
+      <c r="J32" s="1" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
@@ -1948,7 +2031,7 @@
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>42</v>
@@ -1965,7 +2048,9 @@
       <c r="I33" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J33" s="1"/>
+      <c r="J33" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
@@ -1974,24 +2059,26 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="I34" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="J34" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
@@ -2000,24 +2087,26 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="I35" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="J35" s="1"/>
+        <v>163</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
@@ -2026,24 +2115,26 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="I36" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J36" s="1"/>
+        <v>167</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
@@ -2052,24 +2143,26 @@
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="I37" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="J37" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
@@ -2078,108 +2171,116 @@
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="I38" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="J38" s="1"/>
+        <v>180</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="I39" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="J39" s="1"/>
+        <v>186</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="I40" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="J40" s="1"/>
+        <v>192</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="I41" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="J41" s="1"/>
+        <v>198</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>219</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2204,49 +2305,47 @@
     <hyperlink ref="C21" r:id="rId19" xr:uid="{1DC2AC75-173F-4208-912A-5BE30B94B2BB}"/>
     <hyperlink ref="C7" r:id="rId20" xr:uid="{72689D77-6463-48F9-BAD5-EA69677A2ABC}"/>
     <hyperlink ref="C8" r:id="rId21" xr:uid="{96C1432B-3514-4B9B-98FF-ED4181F9F0D2}"/>
-    <hyperlink ref="D22" r:id="rId22" xr:uid="{193F0814-2FA1-445B-A0A1-9B062D5AE6DE}"/>
-    <hyperlink ref="D23" r:id="rId23" xr:uid="{C206515D-7BB0-43D2-8EBF-64C0913FF3E3}"/>
-    <hyperlink ref="D24" r:id="rId24" xr:uid="{683E73AE-13AA-4FCA-B1BB-B72E4466A19A}"/>
-    <hyperlink ref="D25" r:id="rId25" xr:uid="{95A715DC-159D-41F7-B1E1-41514866C6C5}"/>
-    <hyperlink ref="C26" r:id="rId26" xr:uid="{CABB43FC-82FB-4D54-AFAB-C785A4B6C2E1}"/>
-    <hyperlink ref="C27" r:id="rId27" xr:uid="{9D3DEE92-CB21-4B8C-AB9E-796D142EC0C6}"/>
-    <hyperlink ref="C28" r:id="rId28" xr:uid="{BE3C191A-C4CF-4C3A-8676-A6645452F400}"/>
-    <hyperlink ref="D28" r:id="rId29" xr:uid="{4BAB3E17-42D9-4FF1-A641-92C853F560D1}"/>
-    <hyperlink ref="D29" r:id="rId30" xr:uid="{60E715BD-4101-48FA-AF30-3CA27F7AB20B}"/>
-    <hyperlink ref="C29" r:id="rId31" xr:uid="{DD9DEA9F-BCCE-4BE1-A13B-42D644B4D150}"/>
-    <hyperlink ref="C30" r:id="rId32" xr:uid="{115BD165-6F3F-4292-9821-3907A872F1A2}"/>
-    <hyperlink ref="D30" r:id="rId33" xr:uid="{DA48F675-15CD-4E56-8673-27244256B7B0}"/>
-    <hyperlink ref="E31" r:id="rId34" xr:uid="{C663B852-A79C-44DC-96E2-616237E0427A}"/>
-    <hyperlink ref="F31" r:id="rId35" xr:uid="{2087401E-35A9-4C0B-8BE6-E10224F91189}"/>
-    <hyperlink ref="G31" r:id="rId36" xr:uid="{0BC2C147-A3B3-484C-84E1-8111377FBAB2}"/>
-    <hyperlink ref="H31" r:id="rId37" xr:uid="{C9EAC0E3-3D98-4522-90F9-84E27C355E2E}"/>
-    <hyperlink ref="D31" r:id="rId38" xr:uid="{52D02672-E7E6-44DD-AC9B-E221EBF0179D}"/>
-    <hyperlink ref="D32" r:id="rId39" xr:uid="{38517B31-4CAC-4C3F-96B8-625871D96DA4}"/>
-    <hyperlink ref="E32" r:id="rId40" xr:uid="{DC98C291-79EB-45D0-8B53-E18B72B36043}"/>
-    <hyperlink ref="F32" r:id="rId41" xr:uid="{9540FAED-77EE-42A9-A8C0-16115543F4B6}"/>
-    <hyperlink ref="G32" r:id="rId42" xr:uid="{0C8727DA-39A6-485D-96F7-31CB03F96CA4}"/>
-    <hyperlink ref="H32" r:id="rId43" xr:uid="{1E9A9F9E-2DC0-4600-B381-106C451E0E44}"/>
-    <hyperlink ref="D33" r:id="rId44" xr:uid="{98BB4C9E-A694-4DC8-8770-4CE7E50F45CB}"/>
-    <hyperlink ref="E33" r:id="rId45" xr:uid="{645AC32E-ADDF-458C-BB57-80872502175B}"/>
-    <hyperlink ref="F33" r:id="rId46" xr:uid="{3CB543F6-1E03-42C1-8206-93DB25A087D6}"/>
-    <hyperlink ref="G33" r:id="rId47" xr:uid="{F0571FC9-CE61-4DDA-B619-42135FEA39DB}"/>
-    <hyperlink ref="H33" r:id="rId48" xr:uid="{3E7C646F-7201-46A4-B994-67B55E3D2BD6}"/>
-    <hyperlink ref="D34" r:id="rId49" xr:uid="{F1AF4ECF-B600-4BD1-ACDF-82E56C595C2D}"/>
-    <hyperlink ref="D35" r:id="rId50" xr:uid="{2E1D21A0-B273-4033-B160-A4BBBAB7141A}"/>
-    <hyperlink ref="D36" r:id="rId51" xr:uid="{D3A890A8-FD6F-434B-BA93-62E224510B2D}"/>
-    <hyperlink ref="D37" r:id="rId52" xr:uid="{AD682E64-E0AD-43D6-B2B0-34BD81C4AB50}"/>
-    <hyperlink ref="D38" r:id="rId53" xr:uid="{7C2DECE1-3354-48F0-A378-D72E5225C3F4}"/>
-    <hyperlink ref="D39" r:id="rId54" xr:uid="{B753947B-7A0D-4A7E-B4BB-15DF1BE1255D}"/>
-    <hyperlink ref="D40" r:id="rId55" xr:uid="{B7CFEED1-6DFD-4D23-965D-07000467A7B0}"/>
-    <hyperlink ref="D41" r:id="rId56" xr:uid="{8DC55A92-A4D1-41B6-BE2E-AB6D002CF0B6}"/>
-    <hyperlink ref="I3" r:id="rId57" xr:uid="{65177DB1-75CF-42D3-A0CE-E0B486B42F12}"/>
-    <hyperlink ref="I4" r:id="rId58" xr:uid="{DF3E8FAE-A7B6-45E6-B234-F273A3C86BD9}"/>
-    <hyperlink ref="I9" r:id="rId59" xr:uid="{92322F55-879C-44F5-B039-B2A2FF4C8E16}"/>
-    <hyperlink ref="I31" r:id="rId60" xr:uid="{7842850C-ECC0-4757-96C1-319E44FF7F3E}"/>
-    <hyperlink ref="I32" r:id="rId61" xr:uid="{0DDB3440-A1A5-4587-8BC5-B9A8100A5099}"/>
-    <hyperlink ref="I33" r:id="rId62" xr:uid="{277F0301-D491-4641-943C-EC3339711215}"/>
+    <hyperlink ref="D24" r:id="rId22" xr:uid="{683E73AE-13AA-4FCA-B1BB-B72E4466A19A}"/>
+    <hyperlink ref="D25" r:id="rId23" xr:uid="{95A715DC-159D-41F7-B1E1-41514866C6C5}"/>
+    <hyperlink ref="C26" r:id="rId24" xr:uid="{CABB43FC-82FB-4D54-AFAB-C785A4B6C2E1}"/>
+    <hyperlink ref="C27" r:id="rId25" xr:uid="{9D3DEE92-CB21-4B8C-AB9E-796D142EC0C6}"/>
+    <hyperlink ref="C28" r:id="rId26" xr:uid="{BE3C191A-C4CF-4C3A-8676-A6645452F400}"/>
+    <hyperlink ref="D28" r:id="rId27" xr:uid="{4BAB3E17-42D9-4FF1-A641-92C853F560D1}"/>
+    <hyperlink ref="D29" r:id="rId28" xr:uid="{60E715BD-4101-48FA-AF30-3CA27F7AB20B}"/>
+    <hyperlink ref="C29" r:id="rId29" xr:uid="{DD9DEA9F-BCCE-4BE1-A13B-42D644B4D150}"/>
+    <hyperlink ref="C30" r:id="rId30" xr:uid="{115BD165-6F3F-4292-9821-3907A872F1A2}"/>
+    <hyperlink ref="D30" r:id="rId31" xr:uid="{DA48F675-15CD-4E56-8673-27244256B7B0}"/>
+    <hyperlink ref="E31" r:id="rId32" xr:uid="{C663B852-A79C-44DC-96E2-616237E0427A}"/>
+    <hyperlink ref="F31" r:id="rId33" xr:uid="{2087401E-35A9-4C0B-8BE6-E10224F91189}"/>
+    <hyperlink ref="G31" r:id="rId34" xr:uid="{0BC2C147-A3B3-484C-84E1-8111377FBAB2}"/>
+    <hyperlink ref="H31" r:id="rId35" xr:uid="{C9EAC0E3-3D98-4522-90F9-84E27C355E2E}"/>
+    <hyperlink ref="D31" r:id="rId36" xr:uid="{52D02672-E7E6-44DD-AC9B-E221EBF0179D}"/>
+    <hyperlink ref="D32" r:id="rId37" xr:uid="{38517B31-4CAC-4C3F-96B8-625871D96DA4}"/>
+    <hyperlink ref="E32" r:id="rId38" xr:uid="{DC98C291-79EB-45D0-8B53-E18B72B36043}"/>
+    <hyperlink ref="F32" r:id="rId39" xr:uid="{9540FAED-77EE-42A9-A8C0-16115543F4B6}"/>
+    <hyperlink ref="G32" r:id="rId40" xr:uid="{0C8727DA-39A6-485D-96F7-31CB03F96CA4}"/>
+    <hyperlink ref="H32" r:id="rId41" xr:uid="{1E9A9F9E-2DC0-4600-B381-106C451E0E44}"/>
+    <hyperlink ref="D33" r:id="rId42" xr:uid="{98BB4C9E-A694-4DC8-8770-4CE7E50F45CB}"/>
+    <hyperlink ref="E33" r:id="rId43" xr:uid="{645AC32E-ADDF-458C-BB57-80872502175B}"/>
+    <hyperlink ref="F33" r:id="rId44" xr:uid="{3CB543F6-1E03-42C1-8206-93DB25A087D6}"/>
+    <hyperlink ref="G33" r:id="rId45" xr:uid="{F0571FC9-CE61-4DDA-B619-42135FEA39DB}"/>
+    <hyperlink ref="H33" r:id="rId46" xr:uid="{3E7C646F-7201-46A4-B994-67B55E3D2BD6}"/>
+    <hyperlink ref="D34" r:id="rId47" xr:uid="{F1AF4ECF-B600-4BD1-ACDF-82E56C595C2D}"/>
+    <hyperlink ref="D35" r:id="rId48" xr:uid="{2E1D21A0-B273-4033-B160-A4BBBAB7141A}"/>
+    <hyperlink ref="D36" r:id="rId49" xr:uid="{D3A890A8-FD6F-434B-BA93-62E224510B2D}"/>
+    <hyperlink ref="D37" r:id="rId50" xr:uid="{AD682E64-E0AD-43D6-B2B0-34BD81C4AB50}"/>
+    <hyperlink ref="D38" r:id="rId51" xr:uid="{7C2DECE1-3354-48F0-A378-D72E5225C3F4}"/>
+    <hyperlink ref="D39" r:id="rId52" xr:uid="{B753947B-7A0D-4A7E-B4BB-15DF1BE1255D}"/>
+    <hyperlink ref="D40" r:id="rId53" xr:uid="{B7CFEED1-6DFD-4D23-965D-07000467A7B0}"/>
+    <hyperlink ref="D41" r:id="rId54" xr:uid="{8DC55A92-A4D1-41B6-BE2E-AB6D002CF0B6}"/>
+    <hyperlink ref="I3" r:id="rId55" xr:uid="{65177DB1-75CF-42D3-A0CE-E0B486B42F12}"/>
+    <hyperlink ref="I4" r:id="rId56" xr:uid="{DF3E8FAE-A7B6-45E6-B234-F273A3C86BD9}"/>
+    <hyperlink ref="I9" r:id="rId57" xr:uid="{92322F55-879C-44F5-B039-B2A2FF4C8E16}"/>
+    <hyperlink ref="I31" r:id="rId58" xr:uid="{7842850C-ECC0-4757-96C1-319E44FF7F3E}"/>
+    <hyperlink ref="I32" r:id="rId59" xr:uid="{0DDB3440-A1A5-4587-8BC5-B9A8100A5099}"/>
+    <hyperlink ref="I33" r:id="rId60" xr:uid="{277F0301-D491-4641-943C-EC3339711215}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId63"/>
+  <pageSetup orientation="portrait" r:id="rId61"/>
 </worksheet>
 </file>
</xml_diff>